<commit_message>
merge Ernest -> master, fix nombre parametro excel
</commit_message>
<xml_diff>
--- a/Parametros.xlsx
+++ b/Parametros.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Apps\Cenfotec\Calidad y Verificación de Software\proyecto\SeleniumTestCases\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="60" windowWidth="12915" windowHeight="5190"/>
   </bookViews>
@@ -36,20 +41,20 @@
     <t>Levi's 511 Jeans</t>
   </si>
   <si>
-    <t>Nokia Lumio 1020</t>
-  </si>
-  <si>
     <t>$349.00</t>
   </si>
   <si>
     <t>$120.00</t>
+  </si>
+  <si>
+    <t>Nokia Lumia 1020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,12 +121,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -163,7 +171,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -195,9 +203,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,6 +255,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -404,19 +448,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -427,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -438,7 +482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -446,18 +490,18 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -470,24 +514,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>